<commit_message>
Added booleanSet to Group
</commit_message>
<xml_diff>
--- a/image/group.xlsx
+++ b/image/group.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="239">
   <si>
     <t>Path</t>
   </si>
@@ -679,6 +679,15 @@
   </si>
   <si>
     <t>The period over which the characteristic is tested; e.g. the patient had an operation during the month of June.</t>
+  </si>
+  <si>
+    <t>Group.characteristic.booleanSet</t>
+  </si>
+  <si>
+    <t>Use booleanSet to define the members of the population, such as Age Ranges, Genders, Settings</t>
+  </si>
+  <si>
+    <t>What code/value pairs define members?</t>
   </si>
   <si>
     <t>Group.member</t>
@@ -879,7 +888,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL34"/>
+  <dimension ref="A1:AL35"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -898,7 +907,7 @@
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="67.56640625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="87.21875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -3889,7 +3898,7 @@
         <v>39</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="K28" t="s" s="2">
         <v>215</v>
@@ -3898,9 +3907,7 @@
         <v>216</v>
       </c>
       <c r="M28" s="2"/>
-      <c r="N28" t="s" s="2">
-        <v>217</v>
-      </c>
+      <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>39</v>
       </c>
@@ -3957,13 +3964,13 @@
         <v>41</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>140</v>
+        <v>39</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>176</v>
+        <v>39</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>218</v>
+        <v>39</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>39</v>
@@ -3974,7 +3981,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -3985,7 +3992,7 @@
         <v>40</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>39</v>
@@ -3997,16 +4004,18 @@
         <v>39</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>179</v>
+        <v>218</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>180</v>
+        <v>219</v>
       </c>
       <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
+      <c r="N29" t="s" s="2">
+        <v>220</v>
+      </c>
       <c r="O29" t="s" s="2">
         <v>39</v>
       </c>
@@ -4054,22 +4063,22 @@
         <v>39</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>181</v>
+        <v>217</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>182</v>
+        <v>221</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>39</v>
@@ -4080,18 +4089,18 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>39</v>
@@ -4103,17 +4112,15 @@
         <v>39</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>94</v>
+        <v>152</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>95</v>
+        <v>179</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>97</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
         <v>39</v>
@@ -4162,13 +4169,13 @@
         <v>39</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>39</v>
@@ -4188,11 +4195,11 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>187</v>
+        <v>93</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
@@ -4205,26 +4212,24 @@
         <v>39</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I31" t="s" s="2">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="J31" t="s" s="2">
         <v>94</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>188</v>
+        <v>95</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="M31" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="N31" t="s" s="2">
-        <v>102</v>
-      </c>
+      <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>39</v>
       </c>
@@ -4272,7 +4277,7 @@
         <v>39</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>40</v>
@@ -4287,7 +4292,7 @@
         <v>39</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>91</v>
+        <v>182</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>39</v>
@@ -4298,39 +4303,43 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>39</v>
+        <v>187</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>223</v>
+        <v>94</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>224</v>
+        <v>188</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
+        <v>189</v>
+      </c>
+      <c r="M32" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="N32" t="s" s="2">
+        <v>102</v>
+      </c>
       <c r="O32" t="s" s="2">
         <v>39</v>
       </c>
@@ -4378,13 +4387,13 @@
         <v>39</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>39</v>
@@ -4393,7 +4402,7 @@
         <v>39</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>39</v>
@@ -4404,7 +4413,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4412,7 +4421,7 @@
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F33" t="s" s="2">
         <v>49</v>
@@ -4427,7 +4436,7 @@
         <v>39</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="K33" t="s" s="2">
         <v>227</v>
@@ -4436,15 +4445,11 @@
         <v>228</v>
       </c>
       <c r="M33" s="2"/>
-      <c r="N33" t="s" s="2">
-        <v>229</v>
-      </c>
+      <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>39</v>
       </c>
-      <c r="P33" t="s" s="2">
-        <v>230</v>
-      </c>
+      <c r="P33" s="2"/>
       <c r="Q33" t="s" s="2">
         <v>39</v>
       </c>
@@ -4488,10 +4493,10 @@
         <v>39</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>49</v>
@@ -4514,7 +4519,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4537,88 +4542,198 @@
         <v>39</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>118</v>
+        <v>211</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="O34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P34" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="Q34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE34" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="AF34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG34" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AH34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL34" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="2">
         <v>234</v>
       </c>
-      <c r="O34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="P34" t="s" s="2">
+      <c r="B35" s="2"/>
+      <c r="C35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F35" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="G35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J35" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="K35" t="s" s="2">
         <v>235</v>
       </c>
-      <c r="Q34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="R34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="S34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="T34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="U34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="V34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="W34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="X34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Y34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Z34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE34" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="AF34" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG34" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AH34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AK34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AL34" t="s" s="2">
+      <c r="L35" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="O35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P35" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="Q35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE35" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="AF35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG35" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AH35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL35" t="s" s="2">
         <v>39</v>
       </c>
     </row>

</xml_diff>